<commit_message>
Se sube ultima version para iniciar proyecto de Gestion Documental Se creó un nuevo testSuite PC_GestionDocumental.rxtst, se agregó DataSource - ValidaFormularios.xlsx
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor - Inspeccion.xlsx
+++ b/Sura/DataSource - Emision Motor - Inspeccion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAAE828-B1F0-45C0-916D-57D1DEF42C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C07F46-2572-4BDA-B423-96BA4A257FE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,25 +213,25 @@
     <t>Anual</t>
   </si>
   <si>
-    <t>26/01/2021</t>
-  </si>
-  <si>
-    <t>RGR005</t>
-  </si>
-  <si>
-    <t>ABCD0RGR005</t>
-  </si>
-  <si>
-    <t>ZXC0987RGR005</t>
-  </si>
-  <si>
-    <t>RGR006</t>
-  </si>
-  <si>
-    <t>ABCD0RGR006</t>
-  </si>
-  <si>
-    <t>ZXC0987RGR006</t>
+    <t>01/02/2021</t>
+  </si>
+  <si>
+    <t>RGR013</t>
+  </si>
+  <si>
+    <t>ABCD0RGR013</t>
+  </si>
+  <si>
+    <t>ZXC0987RGR013</t>
+  </si>
+  <si>
+    <t>RGR014</t>
+  </si>
+  <si>
+    <t>ABCD0RGR014</t>
+  </si>
+  <si>
+    <t>ZXC0987RGR014</t>
   </si>
 </sst>
 </file>
@@ -331,56 +331,7 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -708,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7:V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1158,7 @@
         <v>18</v>
       </c>
       <c r="O7">
-        <v>2005</v>
+        <v>2015</v>
       </c>
       <c r="P7" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
se agregó en script EmisionMotor la condición para emiti SinAsistenciaMecanica
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor - Inspeccion.xlsx
+++ b/Sura/DataSource - Emision Motor - Inspeccion.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD5722C-A916-45AE-AEB2-5A32EC142E4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4646F9B-365D-46B4-AFBA-9A1F9173BD12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="72">
   <si>
     <t>Usuario</t>
   </si>
@@ -192,27 +200,6 @@
     <t>Anual</t>
   </si>
   <si>
-    <t>01/02/2021</t>
-  </si>
-  <si>
-    <t>RGR013</t>
-  </si>
-  <si>
-    <t>ABCD0RGR013</t>
-  </si>
-  <si>
-    <t>ZXC0987RGR013</t>
-  </si>
-  <si>
-    <t>RGR014</t>
-  </si>
-  <si>
-    <t>ABCD0RGR014</t>
-  </si>
-  <si>
-    <t>ZXC0987RGR014</t>
-  </si>
-  <si>
     <t>03/02/2021</t>
   </si>
   <si>
@@ -232,6 +219,36 @@
   </si>
   <si>
     <t>ZXC0987RPR005</t>
+  </si>
+  <si>
+    <t>SinAsistenciaMecanica</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>PRU004</t>
+  </si>
+  <si>
+    <t>ABCD0PRU004</t>
+  </si>
+  <si>
+    <t>ZXC0987PRU004</t>
+  </si>
+  <si>
+    <t>PRU005</t>
+  </si>
+  <si>
+    <t>ABCD0PRU005</t>
+  </si>
+  <si>
+    <t>ZXC0987PRU005</t>
+  </si>
+  <si>
+    <t>05/02/2021</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -657,616 +674,656 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="75" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="75" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>14</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>15</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>30</v>
       </c>
+      <c r="Z1" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>1785991583</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2302</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>18</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>2015</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>350901</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>29</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>56</v>
+      </c>
+      <c r="V2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z2" t="s">
         <v>63</v>
       </c>
-      <c r="U2" t="s">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1785991583</v>
+      </c>
+      <c r="G3">
+        <v>2302</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3">
+        <v>2003</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3">
+        <v>350900</v>
+      </c>
+      <c r="T3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" t="s">
+        <v>59</v>
+      </c>
+      <c r="V3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2551825244</v>
+      </c>
+      <c r="G4">
+        <v>2302</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4">
+        <v>2003</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4">
+        <v>350900</v>
+      </c>
+      <c r="T4" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2551825244</v>
+      </c>
+      <c r="G5">
+        <v>2302</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5">
+        <v>2008</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5">
+        <v>350901</v>
+      </c>
+      <c r="T5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U5" t="s">
+        <v>43</v>
+      </c>
+      <c r="V5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2551825244</v>
+      </c>
+      <c r="G6">
+        <v>2302</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6">
+        <v>2005</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6">
+        <v>350901</v>
+      </c>
+      <c r="T6" t="s">
+        <v>29</v>
+      </c>
+      <c r="U6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V6" t="s">
+        <v>47</v>
+      </c>
+      <c r="W6" t="s">
+        <v>50</v>
+      </c>
+      <c r="X6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="4">
+        <v>7557632631</v>
+      </c>
+      <c r="G7">
+        <v>2302</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7">
+        <v>2015</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7">
+        <v>350901</v>
+      </c>
+      <c r="T7" t="s">
+        <v>29</v>
+      </c>
+      <c r="U7" t="s">
+        <v>64</v>
+      </c>
+      <c r="V7" t="s">
         <v>65</v>
       </c>
-      <c r="V2" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="W7" t="s">
+        <v>66</v>
+      </c>
+      <c r="X7" t="s">
         <v>24</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y7" t="s">
         <v>26</v>
       </c>
+      <c r="Z7" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="8" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1785991583</v>
-      </c>
-      <c r="F3">
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="4">
+        <v>7557632631</v>
+      </c>
+      <c r="G8">
         <v>2302</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H8" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I8" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="K8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" t="s">
         <v>17</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N8" t="s">
         <v>18</v>
       </c>
-      <c r="O3">
+      <c r="P8">
         <v>2003</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q8" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R8" t="s">
         <v>20</v>
       </c>
-      <c r="R3">
+      <c r="S8">
         <v>350900</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T8" t="s">
         <v>27</v>
       </c>
-      <c r="T3" t="s">
-        <v>66</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="U8" t="s">
         <v>67</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V8" t="s">
         <v>68</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W8" t="s">
+        <v>69</v>
+      </c>
+      <c r="X8" t="s">
         <v>24</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y8" t="s">
         <v>25</v>
       </c>
+      <c r="Z8" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2551825244</v>
-      </c>
-      <c r="F4">
-        <v>2302</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4">
-        <v>2003</v>
-      </c>
-      <c r="P4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4">
-        <v>350900</v>
-      </c>
-      <c r="S4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" t="s">
-        <v>45</v>
-      </c>
-      <c r="V4" t="s">
-        <v>48</v>
-      </c>
-      <c r="W4" t="s">
-        <v>24</v>
-      </c>
-      <c r="X4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2551825244</v>
-      </c>
-      <c r="F5">
-        <v>2302</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5">
-        <v>2008</v>
-      </c>
-      <c r="P5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>20</v>
-      </c>
-      <c r="R5">
-        <v>350901</v>
-      </c>
-      <c r="S5" t="s">
-        <v>28</v>
-      </c>
-      <c r="T5" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" t="s">
-        <v>46</v>
-      </c>
-      <c r="V5" t="s">
-        <v>49</v>
-      </c>
-      <c r="W5" t="s">
-        <v>24</v>
-      </c>
-      <c r="X5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2551825244</v>
-      </c>
-      <c r="F6">
-        <v>2302</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6">
-        <v>2005</v>
-      </c>
-      <c r="P6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6">
-        <v>350901</v>
-      </c>
-      <c r="S6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T6" t="s">
-        <v>44</v>
-      </c>
-      <c r="U6" t="s">
-        <v>47</v>
-      </c>
-      <c r="V6" t="s">
-        <v>50</v>
-      </c>
-      <c r="W6" t="s">
-        <v>24</v>
-      </c>
-      <c r="X6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="4">
-        <v>7557632631</v>
-      </c>
-      <c r="F7">
-        <v>2302</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7">
-        <v>2015</v>
-      </c>
-      <c r="P7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>20</v>
-      </c>
-      <c r="R7">
-        <v>350901</v>
-      </c>
-      <c r="S7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T7" t="s">
-        <v>56</v>
-      </c>
-      <c r="U7" t="s">
-        <v>57</v>
-      </c>
-      <c r="V7" t="s">
-        <v>58</v>
-      </c>
-      <c r="W7" t="s">
-        <v>24</v>
-      </c>
-      <c r="X7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="4">
-        <v>7557632631</v>
-      </c>
-      <c r="F8">
-        <v>2302</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8">
-        <v>2003</v>
-      </c>
-      <c r="P8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>20</v>
-      </c>
-      <c r="R8">
-        <v>350900</v>
-      </c>
-      <c r="S8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T8" t="s">
-        <v>59</v>
-      </c>
-      <c r="U8" t="s">
-        <v>60</v>
-      </c>
-      <c r="V8" t="s">
-        <v>61</v>
-      </c>
-      <c r="W8" t="s">
-        <v>24</v>
-      </c>
-      <c r="X8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="E9" s="3"/>
-      <c r="K9" s="2"/>
+    <row r="9" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
+      <c r="F9" s="3"/>
+      <c r="L9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E9">
+  <conditionalFormatting sqref="F9">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Fallo"</formula>
     </cfRule>
@@ -1277,7 +1334,7 @@
       <formula>"Ejecutado OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
+  <conditionalFormatting sqref="F9">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No OK"</formula>
     </cfRule>
@@ -1286,13 +1343,13 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{10528CBD-F1C8-451F-8C44-67A5E71543CB}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{B87C8C0D-0FC1-4675-990B-4D4A2C29BFA8}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{AD53A963-934B-4F54-9DBD-4DDEAFB1AD98}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{E83F1668-BEE1-497A-A509-4240F2EFEAE9}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{89E88914-314C-4241-9288-A14F53413B69}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{76010F62-F922-44FE-8B46-52D1C9B471C9}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{10528CBD-F1C8-451F-8C44-67A5E71543CB}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{B87C8C0D-0FC1-4675-990B-4D4A2C29BFA8}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{AD53A963-934B-4F54-9DBD-4DDEAFB1AD98}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{E83F1668-BEE1-497A-A509-4240F2EFEAE9}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{89E88914-314C-4241-9288-A14F53413B69}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{76010F62-F922-44FE-8B46-52D1C9B471C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
se agregó también la condición de 0Km en el script de EmisionMotor, se agregó una columna en Es0Km en el DataSource - Emision Motor.xlsx
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor - Inspeccion.xlsx
+++ b/Sura/DataSource - Emision Motor - Inspeccion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4646F9B-365D-46B4-AFBA-9A1F9173BD12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4F8ABA-5721-4C26-9A2B-EAA306F6589D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -245,10 +245,10 @@
     <t>ZXC0987PRU005</t>
   </si>
   <si>
-    <t>05/02/2021</t>
-  </si>
-  <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>08/02/2021</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -1197,7 +1197,7 @@
         <v>54</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M7" t="s">
         <v>17</v>
@@ -1274,7 +1274,7 @@
         <v>54</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M8" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
se crearon los testRun para EmisionMotorAnswer y EmisionMotorAsist0Km
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor - Inspeccion.xlsx
+++ b/Sura/DataSource - Emision Motor - Inspeccion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4F8ABA-5721-4C26-9A2B-EAA306F6589D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D65AB05-4CAD-4946-BB01-A3B8AA84CD28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Agrego logueo de la info de los esquemas de inspección en las emisiones y data de los mismos
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor - Inspeccion.xlsx
+++ b/Sura/DataSource - Emision Motor - Inspeccion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA0296D-263D-4F4E-A6AF-85217B286C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C650680B-1929-44FF-A937-FC17A13D5AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="109">
   <si>
     <t>Usuario</t>
   </si>
@@ -167,22 +159,199 @@
     <t>07/04/2022</t>
   </si>
   <si>
-    <t>RGA004</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA004</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA004</t>
-  </si>
-  <si>
-    <t>RGA005</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA005</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA005</t>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>B - Resp. Civil-Robo/Incendio Total Daños Totales por Accidente</t>
+  </si>
+  <si>
+    <t>Global Solution</t>
+  </si>
+  <si>
+    <t>TR - Todo Riesgo Franquicia Fija</t>
+  </si>
+  <si>
+    <t>Interior</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Panattoni</t>
+  </si>
+  <si>
+    <t>Aon Risk Services Arg Sa-Banca Seguros</t>
+  </si>
+  <si>
+    <t>Prenda</t>
+  </si>
+  <si>
+    <t>NumEsquema</t>
+  </si>
+  <si>
+    <t>NombreEsquema</t>
+  </si>
+  <si>
+    <t>Petrini</t>
+  </si>
+  <si>
+    <t>WAM</t>
+  </si>
+  <si>
+    <t>A - Responsabilidad Civil Unicamente</t>
+  </si>
+  <si>
+    <t>MJK048</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA048</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA048</t>
+  </si>
+  <si>
+    <t>MJK049</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA049</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA049</t>
+  </si>
+  <si>
+    <t>MJK050</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA050</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA050</t>
+  </si>
+  <si>
+    <t>MJK051</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA051</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA051</t>
+  </si>
+  <si>
+    <t>MJK052</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA052</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA052</t>
+  </si>
+  <si>
+    <t>MJK053</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA053</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA053</t>
+  </si>
+  <si>
+    <t>MJK054</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA054</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA054</t>
+  </si>
+  <si>
+    <t>MJK055</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA055</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA055</t>
+  </si>
+  <si>
+    <t>MJK056</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA056</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA056</t>
+  </si>
+  <si>
+    <t>MJK057</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA057</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA057</t>
+  </si>
+  <si>
+    <t>MJK058</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA058</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA058</t>
+  </si>
+  <si>
+    <t>Marsh S.A.</t>
+  </si>
+  <si>
+    <t>MJK061</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA061</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA061</t>
+  </si>
+  <si>
+    <t>MJK062</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA062</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA062</t>
+  </si>
+  <si>
+    <t>MJK063</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA063</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA063</t>
+  </si>
+  <si>
+    <t>Makler</t>
+  </si>
+  <si>
+    <t>Interior Black</t>
+  </si>
+  <si>
+    <t>MJK064</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA064</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA064</t>
+  </si>
+  <si>
+    <t>MJK065</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA065</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA065</t>
   </si>
 </sst>
 </file>
@@ -526,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,25 +709,26 @@
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="20.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="75" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.85546875" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -584,61 +754,67 @@
         <v>22</v>
       </c>
       <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>10</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>13</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>14</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -663,59 +839,65 @@
       <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2">
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2">
         <v>2015</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>19</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>20</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>1380000</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>28</v>
       </c>
-      <c r="U2" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" t="s">
-        <v>45</v>
-      </c>
       <c r="W2" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="X2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z2" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -740,55 +922,1139 @@
       <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>17</v>
       </c>
-      <c r="N3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3">
+      <c r="P3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3">
         <v>2003</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>19</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>20</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>1380000</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>27</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G4">
+        <v>3762</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4">
+        <v>2008</v>
+      </c>
+      <c r="S4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4">
+        <v>1380000</v>
+      </c>
+      <c r="V4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" t="s">
+        <v>64</v>
+      </c>
+      <c r="X4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G5">
+        <v>3762</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5">
+        <v>2018</v>
+      </c>
+      <c r="S5" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U5">
+        <v>1380000</v>
+      </c>
+      <c r="V5" t="s">
         <v>47</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W5" t="s">
+        <v>67</v>
+      </c>
+      <c r="X5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G6">
+        <v>9125</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
         <v>48</v>
       </c>
-      <c r="W3" t="s">
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6">
+        <v>2020</v>
+      </c>
+      <c r="S6" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6">
+        <v>1380000</v>
+      </c>
+      <c r="V6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" t="s">
+        <v>70</v>
+      </c>
+      <c r="X6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G7">
+        <v>9125</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7">
+        <v>2020</v>
+      </c>
+      <c r="S7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T7" t="s">
+        <v>20</v>
+      </c>
+      <c r="U7">
+        <v>1380000</v>
+      </c>
+      <c r="V7" t="s">
+        <v>47</v>
+      </c>
+      <c r="W7" t="s">
+        <v>73</v>
+      </c>
+      <c r="X7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G8">
+        <v>2875</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8">
+        <v>2020</v>
+      </c>
+      <c r="S8" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8">
+        <v>1380000</v>
+      </c>
+      <c r="V8" t="s">
+        <v>47</v>
+      </c>
+      <c r="W8" t="s">
+        <v>76</v>
+      </c>
+      <c r="X8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G9">
+        <v>2875</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" t="s">
+        <v>18</v>
+      </c>
+      <c r="R9">
+        <v>2003</v>
+      </c>
+      <c r="S9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9">
+        <v>1380000</v>
+      </c>
+      <c r="V9" t="s">
+        <v>47</v>
+      </c>
+      <c r="W9" t="s">
+        <v>79</v>
+      </c>
+      <c r="X9" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G10">
+        <v>3336</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10">
+        <v>2019</v>
+      </c>
+      <c r="S10" t="s">
+        <v>19</v>
+      </c>
+      <c r="T10" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10">
+        <v>1380000</v>
+      </c>
+      <c r="V10" t="s">
+        <v>28</v>
+      </c>
+      <c r="W10" t="s">
+        <v>82</v>
+      </c>
+      <c r="X10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G11">
+        <v>3336</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" t="s">
+        <v>39</v>
+      </c>
+      <c r="O11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" t="s">
+        <v>18</v>
+      </c>
+      <c r="R11">
+        <v>2008</v>
+      </c>
+      <c r="S11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T11" t="s">
+        <v>20</v>
+      </c>
+      <c r="U11">
+        <v>1380000</v>
+      </c>
+      <c r="V11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W11" t="s">
+        <v>85</v>
+      </c>
+      <c r="X11" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G12">
+        <v>2594</v>
+      </c>
+      <c r="H12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" t="s">
+        <v>18</v>
+      </c>
+      <c r="R12">
+        <v>2008</v>
+      </c>
+      <c r="S12" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12" t="s">
+        <v>20</v>
+      </c>
+      <c r="U12">
+        <v>1380000</v>
+      </c>
+      <c r="V12" t="s">
+        <v>57</v>
+      </c>
+      <c r="W12" t="s">
+        <v>88</v>
+      </c>
+      <c r="X12" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G13">
+        <v>2594</v>
+      </c>
+      <c r="H13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13" t="s">
+        <v>18</v>
+      </c>
+      <c r="R13">
+        <v>2003</v>
+      </c>
+      <c r="S13" t="s">
+        <v>19</v>
+      </c>
+      <c r="T13" t="s">
+        <v>20</v>
+      </c>
+      <c r="U13">
+        <v>1380000</v>
+      </c>
+      <c r="V13" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13" t="s">
+        <v>92</v>
+      </c>
+      <c r="X13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G14">
+        <v>2650</v>
+      </c>
+      <c r="H14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
         <v>49</v>
       </c>
-      <c r="X3" t="s">
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" t="s">
+        <v>17</v>
+      </c>
+      <c r="P14" t="s">
+        <v>18</v>
+      </c>
+      <c r="R14">
+        <v>2017</v>
+      </c>
+      <c r="S14" t="s">
+        <v>19</v>
+      </c>
+      <c r="T14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U14">
+        <v>1380000</v>
+      </c>
+      <c r="V14" t="s">
+        <v>27</v>
+      </c>
+      <c r="W14" t="s">
+        <v>95</v>
+      </c>
+      <c r="X14" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z14" t="s">
         <v>24</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA14" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G15">
+        <v>2650</v>
+      </c>
+      <c r="H15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" t="s">
+        <v>17</v>
+      </c>
+      <c r="P15" t="s">
+        <v>18</v>
+      </c>
+      <c r="R15">
+        <v>2018</v>
+      </c>
+      <c r="S15" t="s">
+        <v>19</v>
+      </c>
+      <c r="T15" t="s">
+        <v>20</v>
+      </c>
+      <c r="U15">
+        <v>1380000</v>
+      </c>
+      <c r="V15" t="s">
+        <v>47</v>
+      </c>
+      <c r="W15" t="s">
+        <v>98</v>
+      </c>
+      <c r="X15" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA15" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G16">
+        <v>3558</v>
+      </c>
+      <c r="H16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>102</v>
+      </c>
+      <c r="K16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" t="s">
+        <v>39</v>
+      </c>
+      <c r="O16" t="s">
+        <v>17</v>
+      </c>
+      <c r="P16" t="s">
+        <v>18</v>
+      </c>
+      <c r="R16">
+        <v>2008</v>
+      </c>
+      <c r="S16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U16">
+        <v>1380000</v>
+      </c>
+      <c r="V16" t="s">
+        <v>45</v>
+      </c>
+      <c r="W16" t="s">
+        <v>103</v>
+      </c>
+      <c r="X16" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2240451788</v>
+      </c>
+      <c r="G17">
+        <v>3558</v>
+      </c>
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17" t="s">
+        <v>102</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17" t="s">
+        <v>18</v>
+      </c>
+      <c r="R17">
+        <v>2002</v>
+      </c>
+      <c r="S17" t="s">
+        <v>19</v>
+      </c>
+      <c r="T17" t="s">
+        <v>20</v>
+      </c>
+      <c r="U17">
+        <v>1380000</v>
+      </c>
+      <c r="V17" t="s">
+        <v>28</v>
+      </c>
+      <c r="W17" t="s">
+        <v>106</v>
+      </c>
+      <c r="X17" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -797,8 +2063,22 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{10528CBD-F1C8-451F-8C44-67A5E71543CB}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{F159C301-5F0C-4A3F-A337-0A5C4077668C}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{291139C5-050B-437C-8807-F4465399D7A6}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{114EF3AA-5C89-425B-93DB-F9CB0381BCC6}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{7D27973E-82D6-49D8-A802-3D44D61AB537}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{1B82ED65-E2E4-44EC-AA14-123A7006D9E4}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{DCBEAD07-64A4-4EBE-A510-1986C33F8ED3}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{83A9437B-37F7-4572-900D-A8D3D32AA3AD}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{EF0EA2D8-A09E-4D04-862D-19FBA7870C65}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{81DC9E2B-70A8-4DF8-BA59-D05DBB6738F7}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{AF2EA717-6487-4D37-96C9-BD4A989FB010}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{29B097FB-7441-479D-9632-46FFF10697B6}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{886748FA-435A-4A9F-BE09-ED80BAACD7C6}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{D4F9007D-3536-4161-81D6-B7B19ED5593F}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{4CCE86AF-5CE7-4E31-8503-AFD9B0539C5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se modifica data para hacer regresión en Preprod (TestRun: Emisiones)
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor - Inspeccion.xlsx
+++ b/Sura/DataSource - Emision Motor - Inspeccion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C650680B-1929-44FF-A937-FC17A13D5AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AB3F09-22CF-4CFA-AC32-6A04FB13C849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,139 +219,139 @@
     <t>ZXC0987RGA049</t>
   </si>
   <si>
-    <t>MJK050</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA050</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA050</t>
-  </si>
-  <si>
-    <t>MJK051</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA051</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA051</t>
-  </si>
-  <si>
-    <t>MJK052</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA052</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA052</t>
-  </si>
-  <si>
-    <t>MJK053</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA053</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA053</t>
-  </si>
-  <si>
-    <t>MJK054</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA054</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA054</t>
-  </si>
-  <si>
-    <t>MJK055</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA055</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA055</t>
-  </si>
-  <si>
-    <t>MJK056</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA056</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA056</t>
-  </si>
-  <si>
-    <t>MJK057</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA057</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA057</t>
-  </si>
-  <si>
-    <t>MJK058</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA058</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA058</t>
-  </si>
-  <si>
     <t>Marsh S.A.</t>
   </si>
   <si>
-    <t>MJK061</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA061</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA061</t>
-  </si>
-  <si>
-    <t>MJK062</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA062</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA062</t>
-  </si>
-  <si>
-    <t>MJK063</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA063</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA063</t>
-  </si>
-  <si>
     <t>Makler</t>
   </si>
   <si>
     <t>Interior Black</t>
   </si>
   <si>
-    <t>MJK064</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA064</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA064</t>
-  </si>
-  <si>
-    <t>MJK065</t>
-  </si>
-  <si>
-    <t>ABCD0RRGA065</t>
-  </si>
-  <si>
-    <t>ZXC0987RGA065</t>
+    <t>MJK066</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA066</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA066</t>
+  </si>
+  <si>
+    <t>MJK067</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA067</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA067</t>
+  </si>
+  <si>
+    <t>MJK068</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA068</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA068</t>
+  </si>
+  <si>
+    <t>MJK069</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA069</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA069</t>
+  </si>
+  <si>
+    <t>MJK070</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA070</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA070</t>
+  </si>
+  <si>
+    <t>MJK071</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA071</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA071</t>
+  </si>
+  <si>
+    <t>MJK072</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA072</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA072</t>
+  </si>
+  <si>
+    <t>MJK073</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA073</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA073</t>
+  </si>
+  <si>
+    <t>MJK074</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA074</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA074</t>
+  </si>
+  <si>
+    <t>MJK075</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA075</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA075</t>
+  </si>
+  <si>
+    <t>MJK076</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA076</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA076</t>
+  </si>
+  <si>
+    <t>MJK077</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA077</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA077</t>
+  </si>
+  <si>
+    <t>MJK078</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA078</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA078</t>
+  </si>
+  <si>
+    <t>MJK079</t>
+  </si>
+  <si>
+    <t>ABCD0RRGA079</t>
+  </si>
+  <si>
+    <t>ZXC0987RGA079</t>
   </si>
 </sst>
 </file>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,6 +981,9 @@
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -1039,13 +1042,13 @@
         <v>45</v>
       </c>
       <c r="W4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="X4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="Y4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="Z4" t="s">
         <v>24</v>
@@ -1058,6 +1061,9 @@
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
@@ -1116,13 +1122,13 @@
         <v>47</v>
       </c>
       <c r="W5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="X5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="Y5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="Z5" t="s">
         <v>24</v>
@@ -1135,6 +1141,9 @@
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -1193,13 +1202,13 @@
         <v>45</v>
       </c>
       <c r="W6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="X6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="Y6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="Z6" t="s">
         <v>24</v>
@@ -1212,6 +1221,9 @@
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>34</v>
       </c>
@@ -1270,13 +1282,13 @@
         <v>47</v>
       </c>
       <c r="W7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="X7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Y7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Z7" t="s">
         <v>24</v>
@@ -1289,6 +1301,9 @@
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -1347,13 +1362,13 @@
         <v>47</v>
       </c>
       <c r="W8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="X8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="Y8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="Z8" t="s">
         <v>24</v>
@@ -1366,6 +1381,9 @@
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
@@ -1424,13 +1442,13 @@
         <v>47</v>
       </c>
       <c r="W9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="X9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="Y9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="Z9" t="s">
         <v>24</v>
@@ -1443,6 +1461,9 @@
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
@@ -1501,13 +1522,13 @@
         <v>28</v>
       </c>
       <c r="W10" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="X10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Y10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Z10" t="s">
         <v>24</v>
@@ -1520,6 +1541,9 @@
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -1578,13 +1602,13 @@
         <v>28</v>
       </c>
       <c r="W11" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="X11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Y11" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="Z11" t="s">
         <v>24</v>
@@ -1597,6 +1621,9 @@
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>34</v>
       </c>
@@ -1616,7 +1643,7 @@
         <v>2594</v>
       </c>
       <c r="H12" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="I12">
         <v>4</v>
@@ -1655,13 +1682,13 @@
         <v>57</v>
       </c>
       <c r="W12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X12" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="Y12" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="Z12" t="s">
         <v>24</v>
@@ -1674,6 +1701,9 @@
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1693,7 +1723,7 @@
         <v>2594</v>
       </c>
       <c r="H13" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="I13">
         <v>4</v>
@@ -1732,13 +1762,13 @@
         <v>45</v>
       </c>
       <c r="W13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="X13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Y13" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Z13" t="s">
         <v>24</v>
@@ -1751,6 +1781,9 @@
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -1770,7 +1803,7 @@
         <v>2650</v>
       </c>
       <c r="H14" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1809,13 +1842,13 @@
         <v>27</v>
       </c>
       <c r="W14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="X14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Y14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Z14" t="s">
         <v>24</v>
@@ -1828,6 +1861,9 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -1847,7 +1883,7 @@
         <v>2650</v>
       </c>
       <c r="H15" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1886,13 +1922,13 @@
         <v>47</v>
       </c>
       <c r="W15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="X15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="Y15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Z15" t="s">
         <v>24</v>
@@ -1905,6 +1941,9 @@
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -1930,7 +1969,7 @@
         <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="K16" t="s">
         <v>13</v>
@@ -1981,7 +2020,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
@@ -2007,7 +2049,7 @@
         <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="K17" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
inicio validacion de anulacion por reemplazo
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor - Inspeccion.xlsx
+++ b/Sura/DataSource - Emision Motor - Inspeccion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C650680B-1929-44FF-A937-FC17A13D5AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2702E91E-6EB2-4E99-AB4C-FE7167056B79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="112">
   <si>
     <t>Usuario</t>
   </si>
@@ -352,6 +352,15 @@
   </si>
   <si>
     <t>ZXC0987RGA065</t>
+  </si>
+  <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
+  </si>
+  <si>
+    <t>gw</t>
   </si>
 </sst>
 </file>
@@ -695,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB17"/>
+  <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,6 +2067,83 @@
         <v>18</v>
       </c>
     </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="3">
+        <v>8684079401</v>
+      </c>
+      <c r="G18">
+        <v>2302</v>
+      </c>
+      <c r="H18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" t="s">
+        <v>17</v>
+      </c>
+      <c r="P18" t="s">
+        <v>18</v>
+      </c>
+      <c r="R18">
+        <v>2015</v>
+      </c>
+      <c r="S18" t="s">
+        <v>19</v>
+      </c>
+      <c r="T18" t="s">
+        <v>20</v>
+      </c>
+      <c r="U18">
+        <v>1380000</v>
+      </c>
+      <c r="V18" t="s">
+        <v>28</v>
+      </c>
+      <c r="W18" t="s">
+        <v>58</v>
+      </c>
+      <c r="X18" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -2077,8 +2163,9 @@
     <hyperlink ref="C15" r:id="rId14" xr:uid="{886748FA-435A-4A9F-BE09-ED80BAACD7C6}"/>
     <hyperlink ref="C16" r:id="rId15" xr:uid="{D4F9007D-3536-4161-81D6-B7B19ED5593F}"/>
     <hyperlink ref="C17" r:id="rId16" xr:uid="{4CCE86AF-5CE7-4E31-8503-AFD9B0539C5D}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{EAECF954-0A2A-4690-B9D2-8018681D2786}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>